<commit_message>
update video display source
</commit_message>
<xml_diff>
--- a/Stm32F7/STM32H723ZGT6_PIN.xlsx
+++ b/Stm32F7/STM32H723ZGT6_PIN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\stm32_git_workspace\stm32_public_workspace\Stm32F7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{386D6101-F907-49E3-A275-84C7225832F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD37D87-DA3F-4257-A67C-9660B2239A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{329B8DDE-580F-4FEB-AB19-42290A552E36}"/>
+    <workbookView xWindow="13125" yWindow="750" windowWidth="11700" windowHeight="11295" xr2:uid="{329B8DDE-580F-4FEB-AB19-42290A552E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>31474</xdr:colOff>
+      <xdr:colOff>31475</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1095,16 +1095,17 @@
   <dimension ref="F12:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T49" sqref="T49"/>
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="9" width="4.140625" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
     <col min="12" max="16" width="4.140625" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="12" spans="6:22" x14ac:dyDescent="0.25">

</xml_diff>